<commit_message>
Verified strassen MxV recursion in excel
</commit_message>
<xml_diff>
--- a/Strassen_math.xlsx
+++ b/Strassen_math.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a1d4ba5a79c43a4d/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbrin\Documents\GitHub\strassen-snn-accel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF2C3B72-4794-4A73-BA13-773617728DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0B9251-0EA6-4697-802A-506026D4739B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-3600" windowWidth="16440" windowHeight="28320" xr2:uid="{612FE5AF-36F0-4BC7-9AAB-A7A5CB9F06BA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{612FE5AF-36F0-4BC7-9AAB-A7A5CB9F06BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="172">
   <si>
     <t>T0</t>
   </si>
@@ -956,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD2F15B-3E04-4767-9F30-A60E758C5944}">
   <dimension ref="E4:AV60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="AM36" sqref="AM36:AS43"/>
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,16 +996,16 @@
         <v>4</v>
       </c>
       <c r="J6">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="K6">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="L6">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="P6" t="s">
         <v>0</v>
@@ -1021,10 +1022,10 @@
       </c>
       <c r="U6" cm="1">
         <f t="array" ref="U6:V7">J6:K7+L8:M9</f>
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="V6">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Y6" t="s">
         <v>19</v>
@@ -1038,49 +1039,49 @@
       </c>
       <c r="AC6">
         <f>U6+V7</f>
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="AE6" t="s">
         <v>33</v>
       </c>
       <c r="AF6">
         <f>Z6*AC6</f>
-        <v>1156</v>
+        <v>34</v>
       </c>
       <c r="AI6">
         <f>AF6+AF9-AF10+AF12</f>
-        <v>460</v>
+        <v>40</v>
       </c>
       <c r="AJ6">
         <f>AF8+AF10</f>
-        <v>408</v>
+        <v>0</v>
       </c>
       <c r="AM6" cm="1">
         <f t="array" ref="AM6:AN7">AI6:AJ7+AI30:AJ31-AI38:AJ39+AI54:AJ55</f>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="AN6">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="AO6" cm="1">
         <f t="array" ref="AO6:AP7">AI22:AJ23+AI38:AJ39</f>
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="AP6">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AS6" cm="1">
         <f t="array" ref="AS6:AV9">MMULT(E6:H9,J6:M9)</f>
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="AT6">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="AU6">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="AV6">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="5:48" x14ac:dyDescent="0.25">
@@ -1097,16 +1098,16 @@
         <v>8</v>
       </c>
       <c r="J7">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="K7">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="L7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="M7">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="Q7">
         <v>20</v>
@@ -1115,10 +1116,10 @@
         <v>22</v>
       </c>
       <c r="U7">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="V7">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="Y7" t="s">
         <v>20</v>
@@ -1132,46 +1133,46 @@
       </c>
       <c r="AC7">
         <f>U6</f>
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="AE7" t="s">
         <v>34</v>
       </c>
       <c r="AF7">
         <f t="shared" ref="AF7:AF12" si="0">Z7*AC7</f>
-        <v>924</v>
+        <v>42</v>
       </c>
       <c r="AI7">
         <f>AF7+AF9</f>
-        <v>748</v>
+        <v>64</v>
       </c>
       <c r="AJ7">
         <f>AF6-AF7+AF8+AF11</f>
-        <v>664</v>
+        <v>0</v>
       </c>
       <c r="AM7">
-        <v>240</v>
+        <v>70</v>
       </c>
       <c r="AN7">
-        <v>214</v>
+        <v>0</v>
       </c>
       <c r="AO7">
-        <v>188</v>
+        <v>0</v>
       </c>
       <c r="AP7">
-        <v>162</v>
+        <v>0</v>
       </c>
       <c r="AS7">
-        <v>240</v>
+        <v>70</v>
       </c>
       <c r="AT7">
-        <v>214</v>
+        <v>0</v>
       </c>
       <c r="AU7">
-        <v>188</v>
+        <v>0</v>
       </c>
       <c r="AV7">
-        <v>162</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="5:48" x14ac:dyDescent="0.25">
@@ -1188,16 +1189,16 @@
         <v>12</v>
       </c>
       <c r="J8">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="K8">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="M8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Y8" t="s">
         <v>21</v>
@@ -1211,40 +1212,40 @@
       </c>
       <c r="AC8">
         <f>V6-V7</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AE8" t="s">
         <v>35</v>
       </c>
       <c r="AF8">
         <f t="shared" si="0"/>
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="AM8" cm="1">
         <f t="array" ref="AM8:AN9">AI14:AJ15+AI30:AJ31</f>
-        <v>400</v>
+        <v>110</v>
       </c>
       <c r="AN8">
-        <v>358</v>
+        <v>0</v>
       </c>
       <c r="AO8" cm="1">
         <f t="array" ref="AO8:AP9">AI6:AJ7-AI14:AJ15+AI22:AJ23+AI46:AJ47</f>
-        <v>316</v>
+        <v>0</v>
       </c>
       <c r="AP8">
-        <v>274</v>
+        <v>0</v>
       </c>
       <c r="AS8">
-        <v>400</v>
+        <v>110</v>
       </c>
       <c r="AT8">
-        <v>358</v>
+        <v>0</v>
       </c>
       <c r="AU8">
-        <v>316</v>
+        <v>0</v>
       </c>
       <c r="AV8">
-        <v>274</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="5:48" x14ac:dyDescent="0.25">
@@ -1264,13 +1265,13 @@
         <v>4</v>
       </c>
       <c r="K9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y9" t="s">
         <v>22</v>
@@ -1284,46 +1285,46 @@
       </c>
       <c r="AC9">
         <f>U7-U6</f>
-        <v>-8</v>
+        <v>1</v>
       </c>
       <c r="AE9" t="s">
         <v>36</v>
       </c>
       <c r="AF9">
         <f t="shared" si="0"/>
-        <v>-176</v>
+        <v>22</v>
       </c>
       <c r="AI9" s="1" t="str">
         <f>DEC2HEX(AI6)</f>
-        <v>1CC</v>
+        <v>28</v>
       </c>
       <c r="AJ9" s="1" t="str">
         <f>DEC2HEX(AJ6)</f>
-        <v>198</v>
+        <v>0</v>
       </c>
       <c r="AM9">
-        <v>560</v>
+        <v>150</v>
       </c>
       <c r="AN9">
-        <v>502</v>
+        <v>0</v>
       </c>
       <c r="AO9">
-        <v>444</v>
+        <v>0</v>
       </c>
       <c r="AP9">
-        <v>386</v>
+        <v>0</v>
       </c>
       <c r="AS9">
-        <v>560</v>
+        <v>150</v>
       </c>
       <c r="AT9">
-        <v>502</v>
+        <v>0</v>
       </c>
       <c r="AU9">
-        <v>444</v>
+        <v>0</v>
       </c>
       <c r="AV9">
-        <v>386</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="5:48" x14ac:dyDescent="0.25">
@@ -1339,22 +1340,22 @@
       </c>
       <c r="AC10">
         <f>V7</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="AE10" t="s">
         <v>37</v>
       </c>
       <c r="AF10">
         <f t="shared" si="0"/>
-        <v>312</v>
+        <v>0</v>
       </c>
       <c r="AI10" s="1" t="str">
         <f>DEC2HEX(AI7)</f>
-        <v>2EC</v>
+        <v>40</v>
       </c>
       <c r="AJ10" s="1" t="str">
         <f>DEC2HEX(AJ7)</f>
-        <v>298</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="5:48" x14ac:dyDescent="0.25">
@@ -1370,30 +1371,30 @@
       </c>
       <c r="AC11">
         <f>U6+V6</f>
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="AE11" t="s">
         <v>38</v>
       </c>
       <c r="AF11">
         <f t="shared" si="0"/>
-        <v>336</v>
+        <v>8</v>
       </c>
       <c r="AM11" s="1" t="str">
         <f>DEC2HEX(AM6)</f>
-        <v>50</v>
+        <v>1E</v>
       </c>
       <c r="AN11" s="1" t="str">
         <f t="shared" ref="AN11:AP11" si="1">DEC2HEX(AN6)</f>
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="AO11" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>3C</v>
+        <v>0</v>
       </c>
       <c r="AP11" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="5:48" x14ac:dyDescent="0.25">
@@ -1409,30 +1410,30 @@
       </c>
       <c r="AC12">
         <f>U7+V7</f>
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="AE12" t="s">
         <v>39</v>
       </c>
       <c r="AF12">
         <f t="shared" si="0"/>
-        <v>-208</v>
+        <v>-16</v>
       </c>
       <c r="AM12" s="1" t="str">
         <f t="shared" ref="AM12:AP12" si="2">DEC2HEX(AM7)</f>
-        <v>F0</v>
+        <v>46</v>
       </c>
       <c r="AN12" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>D6</v>
+        <v>0</v>
       </c>
       <c r="AO12" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>BC</v>
+        <v>0</v>
       </c>
       <c r="AP12" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>A2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="5:48" x14ac:dyDescent="0.25">
@@ -1441,19 +1442,19 @@
       </c>
       <c r="AM13" s="1" t="str">
         <f t="shared" ref="AM13:AP13" si="3">DEC2HEX(AM8)</f>
-        <v>190</v>
+        <v>6E</v>
       </c>
       <c r="AN13" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>166</v>
+        <v>0</v>
       </c>
       <c r="AO13" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>13C</v>
+        <v>0</v>
       </c>
       <c r="AP13" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>112</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="5:48" x14ac:dyDescent="0.25">
@@ -1472,10 +1473,10 @@
       </c>
       <c r="U14" cm="1">
         <f t="array" ref="U14:V15">J6:K7</f>
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="V14">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="Y14" t="s">
         <v>40</v>
@@ -1489,38 +1490,38 @@
       </c>
       <c r="AC14">
         <f>U14+V15</f>
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="AE14" t="s">
         <v>61</v>
       </c>
       <c r="AF14">
         <f>Z14*AC14</f>
-        <v>1350</v>
+        <v>50</v>
       </c>
       <c r="AI14">
         <f>AF14+AF17-AF18+AF20</f>
-        <v>584</v>
+        <v>64</v>
       </c>
       <c r="AJ14">
         <f>AF16+AF18</f>
-        <v>542</v>
+        <v>0</v>
       </c>
       <c r="AM14" s="1" t="str">
         <f t="shared" ref="AM14:AP14" si="4">DEC2HEX(AM9)</f>
-        <v>230</v>
+        <v>96</v>
       </c>
       <c r="AN14" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>1F6</v>
+        <v>0</v>
       </c>
       <c r="AO14" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>1BC</v>
+        <v>0</v>
       </c>
       <c r="AP14" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>182</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="5:48" x14ac:dyDescent="0.25">
@@ -1531,10 +1532,10 @@
         <v>30</v>
       </c>
       <c r="U15">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="V15">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="Y15" t="s">
         <v>41</v>
@@ -1548,22 +1549,22 @@
       </c>
       <c r="AC15">
         <f>U14</f>
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="AE15" t="s">
         <v>62</v>
       </c>
       <c r="AF15">
         <f t="shared" ref="AF15:AF20" si="5">Z15*AC15</f>
-        <v>928</v>
+        <v>58</v>
       </c>
       <c r="AI15">
         <f>AF15+AF17</f>
-        <v>808</v>
+        <v>88</v>
       </c>
       <c r="AJ15">
         <f>AF14-AF15+AF16+AF19</f>
-        <v>750</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="5:48" x14ac:dyDescent="0.25">
@@ -1579,14 +1580,14 @@
       </c>
       <c r="AC16">
         <f>V14-V15</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AE16" t="s">
         <v>63</v>
       </c>
       <c r="AF16">
         <f t="shared" si="5"/>
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="16:36" x14ac:dyDescent="0.25">
@@ -1602,22 +1603,22 @@
       </c>
       <c r="AC17">
         <f>U15-U14</f>
-        <v>-4</v>
+        <v>1</v>
       </c>
       <c r="AE17" t="s">
         <v>64</v>
       </c>
       <c r="AF17">
         <f t="shared" si="5"/>
-        <v>-120</v>
+        <v>30</v>
       </c>
       <c r="AI17" s="1" t="str">
         <f>DEC2HEX(AI14)</f>
-        <v>248</v>
+        <v>40</v>
       </c>
       <c r="AJ17" s="1" t="str">
         <f>DEC2HEX(AJ14)</f>
-        <v>21E</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="16:36" x14ac:dyDescent="0.25">
@@ -1633,22 +1634,22 @@
       </c>
       <c r="AC18">
         <f>V15</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="AE18" t="s">
         <v>65</v>
       </c>
       <c r="AF18">
         <f t="shared" si="5"/>
-        <v>462</v>
+        <v>0</v>
       </c>
       <c r="AI18" s="1" t="str">
         <f>DEC2HEX(AI15)</f>
-        <v>328</v>
+        <v>58</v>
       </c>
       <c r="AJ18" s="1" t="str">
         <f>DEC2HEX(AJ15)</f>
-        <v>2EE</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="16:36" x14ac:dyDescent="0.25">
@@ -1664,14 +1665,14 @@
       </c>
       <c r="AC19">
         <f>U14+V14</f>
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="AE19" t="s">
         <v>66</v>
       </c>
       <c r="AF19">
         <f t="shared" si="5"/>
-        <v>248</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="16:36" x14ac:dyDescent="0.25">
@@ -1687,14 +1688,14 @@
       </c>
       <c r="AC20">
         <f>U15+V15</f>
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="AE20" t="s">
         <v>67</v>
       </c>
       <c r="AF20">
         <f t="shared" si="5"/>
-        <v>-184</v>
+        <v>-16</v>
       </c>
     </row>
     <row r="21" spans="16:36" x14ac:dyDescent="0.25">
@@ -1718,10 +1719,10 @@
       </c>
       <c r="U22" cm="1">
         <f t="array" ref="U22:V23">L6:M7-L8:M9</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="V22">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Y22" t="s">
         <v>47</v>
@@ -1735,22 +1736,22 @@
       </c>
       <c r="AC22">
         <f>U22+V23</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="AE22" t="s">
         <v>75</v>
       </c>
       <c r="AF22">
         <f>Z22*AC22</f>
-        <v>112</v>
+        <v>0</v>
       </c>
       <c r="AI22">
         <f>AF22+AF25-AF26+AF28</f>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AJ22">
         <f>AF24+AF26</f>
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="16:36" x14ac:dyDescent="0.25">
@@ -1761,10 +1762,10 @@
         <v>6</v>
       </c>
       <c r="U23">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="V23">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Y23" t="s">
         <v>55</v>
@@ -1778,22 +1779,22 @@
       </c>
       <c r="AC23">
         <f>U22</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AE23" t="s">
         <v>76</v>
       </c>
       <c r="AF23">
         <f t="shared" ref="AF23:AF28" si="6">Z23*AC23</f>
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="AI23">
         <f>AF23+AF25</f>
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="AJ23">
         <f>AF22-AF23+AF24+AF27</f>
-        <v>88</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="16:36" x14ac:dyDescent="0.25">
@@ -1843,11 +1844,11 @@
       </c>
       <c r="AI25" s="1" t="str">
         <f>DEC2HEX(AI22)</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="AJ25" s="1" t="str">
         <f>DEC2HEX(AJ22)</f>
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="16:36" x14ac:dyDescent="0.25">
@@ -1863,22 +1864,22 @@
       </c>
       <c r="AC26">
         <f>V23</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AE26" t="s">
         <v>79</v>
       </c>
       <c r="AF26">
         <f t="shared" si="6"/>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AI26" s="1" t="str">
         <f>DEC2HEX(AI23)</f>
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="AJ26" s="1" t="str">
         <f>DEC2HEX(AJ23)</f>
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="16:36" x14ac:dyDescent="0.25">
@@ -1894,14 +1895,14 @@
       </c>
       <c r="AC27">
         <f>U22+V22</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="AE27" t="s">
         <v>80</v>
       </c>
       <c r="AF27">
         <f t="shared" si="6"/>
-        <v>64</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="16:36" x14ac:dyDescent="0.25">
@@ -1917,14 +1918,14 @@
       </c>
       <c r="AC28">
         <f>U23+V23</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="AE28" t="s">
         <v>81</v>
       </c>
       <c r="AF28">
         <f t="shared" si="6"/>
-        <v>-64</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="16:36" x14ac:dyDescent="0.25">
@@ -1948,10 +1949,10 @@
       </c>
       <c r="U30" cm="1">
         <f t="array" ref="U30:V31">J8:K9-J6:K7</f>
-        <v>-8</v>
+        <v>2</v>
       </c>
       <c r="V30">
-        <v>-8</v>
+        <v>0</v>
       </c>
       <c r="Y30" t="s">
         <v>82</v>
@@ -1965,22 +1966,22 @@
       </c>
       <c r="AC30">
         <f>U30+V31</f>
-        <v>-16</v>
+        <v>2</v>
       </c>
       <c r="AE30" t="s">
         <v>96</v>
       </c>
       <c r="AF30">
         <f>Z30*AC30</f>
-        <v>-432</v>
+        <v>54</v>
       </c>
       <c r="AI30">
         <f>AF30+AF33-AF34+AF36</f>
-        <v>-184</v>
+        <v>46</v>
       </c>
       <c r="AJ30">
         <f>AF32+AF34</f>
-        <v>-184</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="16:36" x14ac:dyDescent="0.25">
@@ -1991,10 +1992,10 @@
         <v>16</v>
       </c>
       <c r="U31">
-        <v>-8</v>
+        <v>2</v>
       </c>
       <c r="V31">
-        <v>-8</v>
+        <v>0</v>
       </c>
       <c r="Y31" t="s">
         <v>83</v>
@@ -2008,22 +2009,22 @@
       </c>
       <c r="AC31">
         <f>U30</f>
-        <v>-8</v>
+        <v>2</v>
       </c>
       <c r="AE31" t="s">
         <v>97</v>
       </c>
       <c r="AF31">
         <f t="shared" ref="AF31:AF36" si="7">Z31*AC31</f>
-        <v>-248</v>
+        <v>62</v>
       </c>
       <c r="AI31">
         <f>AF31+AF33</f>
-        <v>-248</v>
+        <v>62</v>
       </c>
       <c r="AJ31">
         <f>AF30-AF31+AF32+AF35</f>
-        <v>-248</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="16:36" x14ac:dyDescent="0.25">
@@ -2073,11 +2074,11 @@
       </c>
       <c r="AI33" s="1" t="str">
         <f>DEC2HEX(AI30)</f>
-        <v>FFFFFFFF48</v>
+        <v>2E</v>
       </c>
       <c r="AJ33" s="1" t="str">
         <f>DEC2HEX(AJ30)</f>
-        <v>FFFFFFFF48</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="16:36" x14ac:dyDescent="0.25">
@@ -2093,22 +2094,22 @@
       </c>
       <c r="AC34">
         <f>V31</f>
-        <v>-8</v>
+        <v>0</v>
       </c>
       <c r="AE34" t="s">
         <v>100</v>
       </c>
       <c r="AF34">
         <f t="shared" si="7"/>
-        <v>-184</v>
+        <v>0</v>
       </c>
       <c r="AI34" s="1" t="str">
         <f>DEC2HEX(AI31)</f>
-        <v>FFFFFFFF08</v>
+        <v>3E</v>
       </c>
       <c r="AJ34" s="1" t="str">
         <f>DEC2HEX(AJ31)</f>
-        <v>FFFFFFFF08</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="16:36" x14ac:dyDescent="0.25">
@@ -2124,14 +2125,14 @@
       </c>
       <c r="AC35">
         <f>U30+V30</f>
-        <v>-16</v>
+        <v>2</v>
       </c>
       <c r="AE35" t="s">
         <v>101</v>
       </c>
       <c r="AF35">
         <f t="shared" si="7"/>
-        <v>-64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="16:36" x14ac:dyDescent="0.25">
@@ -2147,14 +2148,14 @@
       </c>
       <c r="AC36">
         <f>U31+V31</f>
-        <v>-16</v>
+        <v>2</v>
       </c>
       <c r="AE36" t="s">
         <v>102</v>
       </c>
       <c r="AF36">
         <f t="shared" si="7"/>
-        <v>64</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="37" spans="16:36" x14ac:dyDescent="0.25">
@@ -2178,10 +2179,10 @@
       </c>
       <c r="U38" cm="1">
         <f t="array" ref="U38:V39">L8:M9</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="V38">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Y38" t="s">
         <v>103</v>
@@ -2195,22 +2196,22 @@
       </c>
       <c r="AC38">
         <f>U38+V39</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AE38" t="s">
         <v>117</v>
       </c>
       <c r="AF38">
         <f>Z38*AC38</f>
-        <v>126</v>
+        <v>0</v>
       </c>
       <c r="AI38">
         <f>AF38+AF41-AF42+AF44</f>
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="AJ38">
         <f>AF40+AF42</f>
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="16:36" x14ac:dyDescent="0.25">
@@ -2221,10 +2222,10 @@
         <v>14</v>
       </c>
       <c r="U39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y39" t="s">
         <v>104</v>
@@ -2238,22 +2239,22 @@
       </c>
       <c r="AC39">
         <f>U38</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AE39" t="s">
         <v>118</v>
       </c>
       <c r="AF39">
         <f t="shared" ref="AF39:AF44" si="8">Z39*AC39</f>
-        <v>156</v>
+        <v>0</v>
       </c>
       <c r="AI39">
         <f>AF39+AF41</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AJ39">
         <f>AF38-AF39+AF40+AF43</f>
-        <v>74</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="16:36" x14ac:dyDescent="0.25">
@@ -2269,14 +2270,14 @@
       </c>
       <c r="AC40">
         <f>V38-V39</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AE40" t="s">
         <v>119</v>
       </c>
       <c r="AF40">
         <f t="shared" si="8"/>
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="16:36" x14ac:dyDescent="0.25">
@@ -2292,22 +2293,22 @@
       </c>
       <c r="AC41">
         <f>U39-U38</f>
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="AE41" t="s">
         <v>120</v>
       </c>
       <c r="AF41">
         <f t="shared" si="8"/>
-        <v>-56</v>
+        <v>0</v>
       </c>
       <c r="AI41" s="1" t="str">
         <f>DEC2HEX(AI38)</f>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AJ41" s="1" t="str">
         <f>DEC2HEX(AJ38)</f>
-        <v>1A</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="16:36" x14ac:dyDescent="0.25">
@@ -2323,22 +2324,22 @@
       </c>
       <c r="AC42">
         <f>V39</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE42" t="s">
         <v>121</v>
       </c>
       <c r="AF42">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AI42" s="1" t="str">
         <f>DEC2HEX(AI39)</f>
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="AJ42" s="1" t="str">
         <f>DEC2HEX(AJ39)</f>
-        <v>4A</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="16:36" x14ac:dyDescent="0.25">
@@ -2354,14 +2355,14 @@
       </c>
       <c r="AC43">
         <f>U38+V38</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="AE43" t="s">
         <v>122</v>
       </c>
       <c r="AF43">
         <f t="shared" si="8"/>
-        <v>88</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="16:36" x14ac:dyDescent="0.25">
@@ -2377,14 +2378,14 @@
       </c>
       <c r="AC44">
         <f>U39+V39</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AE44" t="s">
         <v>123</v>
       </c>
       <c r="AF44">
         <f t="shared" si="8"/>
-        <v>-24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="16:36" x14ac:dyDescent="0.25">
@@ -2408,10 +2409,10 @@
       </c>
       <c r="U46" cm="1">
         <f t="array" ref="U46:V47">J6:K7+L6:M7</f>
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="V46">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="Y46" t="s">
         <v>124</v>
@@ -2425,22 +2426,22 @@
       </c>
       <c r="AC46">
         <f>U46+V47</f>
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="AE46" t="s">
         <v>138</v>
       </c>
       <c r="AF46">
         <f>Z46*AC46</f>
-        <v>800</v>
+        <v>16</v>
       </c>
       <c r="AI46">
         <f>AF46+AF49-AF50+AF52</f>
-        <v>416</v>
+        <v>24</v>
       </c>
       <c r="AJ46">
         <f>AF48+AF50</f>
-        <v>384</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="16:36" x14ac:dyDescent="0.25">
@@ -2451,10 +2452,10 @@
         <v>8</v>
       </c>
       <c r="U47">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="V47">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Y47" t="s">
         <v>125</v>
@@ -2468,22 +2469,22 @@
       </c>
       <c r="AC47">
         <f>U46</f>
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="AE47" t="s">
         <v>139</v>
       </c>
       <c r="AF47">
         <f t="shared" ref="AF47:AF52" si="9">Z47*AC47</f>
-        <v>480</v>
+        <v>16</v>
       </c>
       <c r="AI47">
         <f>AF47+AF49</f>
-        <v>416</v>
+        <v>24</v>
       </c>
       <c r="AJ47">
         <f>AF46-AF47+AF48+AF51</f>
-        <v>384</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="16:36" x14ac:dyDescent="0.25">
@@ -2499,14 +2500,14 @@
       </c>
       <c r="AC48">
         <f>V46-V47</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AE48" t="s">
         <v>140</v>
       </c>
       <c r="AF48">
         <f t="shared" si="9"/>
-        <v>64</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="16:36" x14ac:dyDescent="0.25">
@@ -2522,22 +2523,22 @@
       </c>
       <c r="AC49">
         <f>U47-U46</f>
-        <v>-8</v>
+        <v>1</v>
       </c>
       <c r="AE49" t="s">
         <v>141</v>
       </c>
       <c r="AF49">
         <f t="shared" si="9"/>
-        <v>-64</v>
+        <v>8</v>
       </c>
       <c r="AI49" s="1" t="str">
         <f>DEC2HEX(AI46)</f>
-        <v>1A0</v>
+        <v>18</v>
       </c>
       <c r="AJ49" s="1" t="str">
         <f>DEC2HEX(AJ46)</f>
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="16:36" x14ac:dyDescent="0.25">
@@ -2553,22 +2554,22 @@
       </c>
       <c r="AC50">
         <f>V47</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AE50" t="s">
         <v>142</v>
       </c>
       <c r="AF50">
         <f t="shared" si="9"/>
-        <v>320</v>
+        <v>0</v>
       </c>
       <c r="AI50" s="1" t="str">
         <f>DEC2HEX(AI47)</f>
-        <v>1A0</v>
+        <v>18</v>
       </c>
       <c r="AJ50" s="1" t="str">
         <f>DEC2HEX(AJ47)</f>
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="16:36" x14ac:dyDescent="0.25">
@@ -2584,7 +2585,7 @@
       </c>
       <c r="AC51">
         <f>U46+V46</f>
-        <v>58</v>
+        <v>1</v>
       </c>
       <c r="AE51" t="s">
         <v>143</v>
@@ -2607,7 +2608,7 @@
       </c>
       <c r="AC52">
         <f>U47+V47</f>
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="AE52" t="s">
         <v>144</v>
@@ -2638,10 +2639,10 @@
       </c>
       <c r="U54" cm="1">
         <f t="array" ref="U54:V55">J8:K9+L8:M9</f>
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="V54">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="Y54" t="s">
         <v>145</v>
@@ -2655,22 +2656,22 @@
       </c>
       <c r="AC54">
         <f>U54+V55</f>
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AE54" t="s">
         <v>159</v>
       </c>
       <c r="AF54">
         <f>Z54*AC54</f>
-        <v>-288</v>
+        <v>-48</v>
       </c>
       <c r="AI54">
         <f>AF54+AF57-AF58+AF60</f>
-        <v>-160</v>
+        <v>-56</v>
       </c>
       <c r="AJ54">
         <f>AF56+AF58</f>
-        <v>-128</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="16:36" x14ac:dyDescent="0.25">
@@ -2681,10 +2682,10 @@
         <v>-8</v>
       </c>
       <c r="U55">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="V55">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Y55" t="s">
         <v>146</v>
@@ -2698,22 +2699,22 @@
       </c>
       <c r="AC55">
         <f>U54</f>
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="AE55" t="s">
         <v>160</v>
       </c>
       <c r="AF55">
         <f t="shared" ref="AF55:AF60" si="10">Z55*AC55</f>
-        <v>-224</v>
+        <v>-48</v>
       </c>
       <c r="AI55">
         <f>AF55+AF57</f>
-        <v>-160</v>
+        <v>-56</v>
       </c>
       <c r="AJ55">
         <f>AF54-AF55+AF56+AF59</f>
-        <v>-128</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="16:36" x14ac:dyDescent="0.25">
@@ -2729,14 +2730,14 @@
       </c>
       <c r="AC56">
         <f>V54-V55</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AE56" t="s">
         <v>161</v>
       </c>
       <c r="AF56">
         <f t="shared" si="10"/>
-        <v>-64</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="16:36" x14ac:dyDescent="0.25">
@@ -2752,22 +2753,22 @@
       </c>
       <c r="AC57">
         <f>U55-U54</f>
-        <v>-8</v>
+        <v>1</v>
       </c>
       <c r="AE57" t="s">
         <v>162</v>
       </c>
       <c r="AF57">
         <f t="shared" si="10"/>
-        <v>64</v>
+        <v>-8</v>
       </c>
       <c r="AI57" s="1" t="str">
         <f>DEC2HEX(AI54)</f>
-        <v>FFFFFFFF60</v>
+        <v>FFFFFFFFC8</v>
       </c>
       <c r="AJ57" s="1" t="str">
         <f>DEC2HEX(AJ54)</f>
-        <v>FFFFFFFF80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="16:36" x14ac:dyDescent="0.25">
@@ -2783,22 +2784,22 @@
       </c>
       <c r="AC58">
         <f>V55</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AE58" t="s">
         <v>163</v>
       </c>
       <c r="AF58">
         <f t="shared" si="10"/>
-        <v>-64</v>
+        <v>0</v>
       </c>
       <c r="AI58" s="1" t="str">
         <f>DEC2HEX(AI55)</f>
-        <v>FFFFFFFF60</v>
+        <v>FFFFFFFFC8</v>
       </c>
       <c r="AJ58" s="1" t="str">
         <f>DEC2HEX(AJ55)</f>
-        <v>FFFFFFFF80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="16:36" x14ac:dyDescent="0.25">
@@ -2814,7 +2815,7 @@
       </c>
       <c r="AC59">
         <f>U54+V54</f>
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="AE59" t="s">
         <v>164</v>
@@ -2837,7 +2838,7 @@
       </c>
       <c r="AC60">
         <f>U55+V55</f>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="AE60" t="s">
         <v>165</v>
@@ -2846,6 +2847,707 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC09DD55-F353-4F19-A23A-AFF11BE70FA5}">
+  <dimension ref="E4:AS58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AO31" sqref="AO31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="5:45" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="5:45" x14ac:dyDescent="0.25">
+      <c r="AH5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>170</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="5:45" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="P6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q6" cm="1">
+        <f t="array" ref="Q6:R7">E8:F9+G8:H9</f>
+        <v>20</v>
+      </c>
+      <c r="R6">
+        <v>22</v>
+      </c>
+      <c r="T6" t="s">
+        <v>10</v>
+      </c>
+      <c r="U6" cm="1">
+        <f t="array" ref="U6:U7">J6:J7</f>
+        <v>1</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z6">
+        <f>Q7+R7</f>
+        <v>58</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC6">
+        <f>U6</f>
+        <v>1</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF6">
+        <f>Z6*AC6</f>
+        <v>58</v>
+      </c>
+      <c r="AI6">
+        <f>AF7+AF9</f>
+        <v>64</v>
+      </c>
+      <c r="AM6" cm="1">
+        <f t="array" ref="AM6:AM7">AI14:AI15+AI30:AI31</f>
+        <v>30</v>
+      </c>
+      <c r="AS6" cm="1">
+        <f t="array" ref="AS6:AS9">MMULT(E6:H9,J6:J9)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="5:45" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+      <c r="H7">
+        <v>8</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="Q7">
+        <v>28</v>
+      </c>
+      <c r="R7">
+        <v>30</v>
+      </c>
+      <c r="U7">
+        <v>2</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z7">
+        <f>Q6</f>
+        <v>20</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC7">
+        <f>U6-U7</f>
+        <v>-1</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF7">
+        <f>Z7*AC7</f>
+        <v>-20</v>
+      </c>
+      <c r="AI7">
+        <f>AF6+AF8</f>
+        <v>88</v>
+      </c>
+      <c r="AM7">
+        <v>70</v>
+      </c>
+      <c r="AS7">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="5:45" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>9</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>11</v>
+      </c>
+      <c r="H8">
+        <v>12</v>
+      </c>
+      <c r="J8">
+        <v>3</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z8">
+        <f>R7</f>
+        <v>30</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC8">
+        <f>U7-U6</f>
+        <v>1</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF8">
+        <f>Z8*AC8</f>
+        <v>30</v>
+      </c>
+      <c r="AM8" cm="1">
+        <f t="array" ref="AM8:AM9">AI6:AI7+AI30:AI31</f>
+        <v>100</v>
+      </c>
+      <c r="AS8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="5:45" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>13</v>
+      </c>
+      <c r="F9">
+        <v>14</v>
+      </c>
+      <c r="G9">
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <v>16</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z9">
+        <f>Q6+R6</f>
+        <v>42</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC9">
+        <f>U7</f>
+        <v>2</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF9">
+        <f>Z9*AC9</f>
+        <v>84</v>
+      </c>
+      <c r="AI9" s="1"/>
+      <c r="AJ9" s="1"/>
+      <c r="AM9">
+        <v>180</v>
+      </c>
+      <c r="AS9">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="5:45" x14ac:dyDescent="0.25">
+      <c r="AI10" s="1"/>
+      <c r="AJ10" s="1"/>
+    </row>
+    <row r="11" spans="5:45" x14ac:dyDescent="0.25">
+      <c r="AM11" s="1"/>
+      <c r="AN11" s="1"/>
+      <c r="AO11" s="1"/>
+      <c r="AP11" s="1"/>
+    </row>
+    <row r="12" spans="5:45" x14ac:dyDescent="0.25">
+      <c r="AM12" s="1"/>
+      <c r="AN12" s="1"/>
+      <c r="AO12" s="1"/>
+      <c r="AP12" s="1"/>
+    </row>
+    <row r="13" spans="5:45" x14ac:dyDescent="0.25">
+      <c r="AH13" t="s">
+        <v>18</v>
+      </c>
+      <c r="AM13" s="1"/>
+      <c r="AN13" s="1"/>
+      <c r="AO13" s="1"/>
+      <c r="AP13" s="1"/>
+    </row>
+    <row r="14" spans="5:45" x14ac:dyDescent="0.25">
+      <c r="P14" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q14" cm="1">
+        <f t="array" ref="Q14:R15">E6:F7</f>
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <v>2</v>
+      </c>
+      <c r="T14" t="s">
+        <v>11</v>
+      </c>
+      <c r="U14" cm="1">
+        <f t="array" ref="U14:U15">J6:J7-J8:J9</f>
+        <v>-2</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z14">
+        <f>Q15+R15</f>
+        <v>11</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC14">
+        <f>U14</f>
+        <v>-2</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF14">
+        <f>Z14*AC14</f>
+        <v>-22</v>
+      </c>
+      <c r="AI14">
+        <f>AF15+AF17</f>
+        <v>-6</v>
+      </c>
+      <c r="AM14" s="1"/>
+      <c r="AN14" s="1"/>
+      <c r="AO14" s="1"/>
+      <c r="AP14" s="1"/>
+    </row>
+    <row r="15" spans="5:45" x14ac:dyDescent="0.25">
+      <c r="Q15">
+        <v>5</v>
+      </c>
+      <c r="R15">
+        <v>6</v>
+      </c>
+      <c r="U15">
+        <v>-2</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z15">
+        <f>Q14</f>
+        <v>1</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC15">
+        <f>U14-U15</f>
+        <v>0</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF15">
+        <f>Z15*AC15</f>
+        <v>0</v>
+      </c>
+      <c r="AI15">
+        <f>AF14+AF16</f>
+        <v>-22</v>
+      </c>
+    </row>
+    <row r="16" spans="5:45" x14ac:dyDescent="0.25">
+      <c r="Y16" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z16">
+        <f>R15</f>
+        <v>6</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC16">
+        <f>U15-U14</f>
+        <v>0</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF16">
+        <f>Z16*AC16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="16:36" x14ac:dyDescent="0.25">
+      <c r="Y17" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z17">
+        <f>Q14+R14</f>
+        <v>3</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC17">
+        <f>U15</f>
+        <v>-2</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF17">
+        <f>Z17*AC17</f>
+        <v>-6</v>
+      </c>
+      <c r="AI17" s="1"/>
+      <c r="AJ17" s="1"/>
+    </row>
+    <row r="18" spans="16:36" x14ac:dyDescent="0.25">
+      <c r="AI18" s="1"/>
+      <c r="AJ18" s="1"/>
+    </row>
+    <row r="21" spans="16:36" x14ac:dyDescent="0.25">
+      <c r="AH21" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="16:36" x14ac:dyDescent="0.25">
+      <c r="P22" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q22" cm="1">
+        <f t="array" ref="Q22:R23">G8:H9</f>
+        <v>11</v>
+      </c>
+      <c r="R22">
+        <v>12</v>
+      </c>
+      <c r="T22" t="s">
+        <v>12</v>
+      </c>
+      <c r="U22" cm="1">
+        <f t="array" ref="U22:U23">J8:J9-J6:J7</f>
+        <v>2</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z22">
+        <f>Q23+R23</f>
+        <v>31</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC22">
+        <f>U22</f>
+        <v>2</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>97</v>
+      </c>
+      <c r="AF22">
+        <f>Z22*AC22</f>
+        <v>62</v>
+      </c>
+      <c r="AI22">
+        <f>AF23+AF25</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="16:36" x14ac:dyDescent="0.25">
+      <c r="Q23">
+        <v>15</v>
+      </c>
+      <c r="R23">
+        <v>16</v>
+      </c>
+      <c r="U23">
+        <v>2</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z23">
+        <f>Q22</f>
+        <v>11</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC23">
+        <f>U22-U23</f>
+        <v>0</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF23">
+        <f>Z23*AC23</f>
+        <v>0</v>
+      </c>
+      <c r="AI23">
+        <f>AF22+AF24</f>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="16:36" x14ac:dyDescent="0.25">
+      <c r="Y24" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z24">
+        <f>R23</f>
+        <v>16</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC24">
+        <f>U23-U22</f>
+        <v>0</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF24">
+        <f>Z24*AC24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="16:36" x14ac:dyDescent="0.25">
+      <c r="Y25" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z25">
+        <f>Q22+R22</f>
+        <v>23</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC25">
+        <f>U23</f>
+        <v>2</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF25">
+        <f>Z25*AC25</f>
+        <v>46</v>
+      </c>
+      <c r="AI25" s="1"/>
+      <c r="AJ25" s="1"/>
+    </row>
+    <row r="26" spans="16:36" x14ac:dyDescent="0.25">
+      <c r="AI26" s="1"/>
+      <c r="AJ26" s="1"/>
+    </row>
+    <row r="29" spans="16:36" x14ac:dyDescent="0.25">
+      <c r="AH29" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="16:36" x14ac:dyDescent="0.25">
+      <c r="P30" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q30" cm="1">
+        <f t="array" ref="Q30:R31">E6:F7+G6:H7</f>
+        <v>4</v>
+      </c>
+      <c r="R30">
+        <v>6</v>
+      </c>
+      <c r="T30" t="s">
+        <v>13</v>
+      </c>
+      <c r="U30" cm="1">
+        <f t="array" ref="U30:U31">J8:J9</f>
+        <v>3</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z30">
+        <f>Q31+R31</f>
+        <v>26</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>111</v>
+      </c>
+      <c r="AC30">
+        <f>U30</f>
+        <v>3</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>118</v>
+      </c>
+      <c r="AF30">
+        <f>Z30*AC30</f>
+        <v>78</v>
+      </c>
+      <c r="AI30">
+        <f>AF31+AF33</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="16:36" x14ac:dyDescent="0.25">
+      <c r="Q31">
+        <v>12</v>
+      </c>
+      <c r="R31">
+        <v>14</v>
+      </c>
+      <c r="U31">
+        <v>4</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z31">
+        <f>Q30</f>
+        <v>4</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC31">
+        <f>U30-U31</f>
+        <v>-1</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>119</v>
+      </c>
+      <c r="AF31">
+        <f>Z31*AC31</f>
+        <v>-4</v>
+      </c>
+      <c r="AI31">
+        <f>AF30+AF32</f>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="16:36" x14ac:dyDescent="0.25">
+      <c r="Y32" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z32">
+        <f>R31</f>
+        <v>14</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>113</v>
+      </c>
+      <c r="AC32">
+        <f>U31-U30</f>
+        <v>1</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF32">
+        <f>Z32*AC32</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="Y33" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z33">
+        <f>Q30+R30</f>
+        <v>10</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC33">
+        <f>U31</f>
+        <v>4</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF33">
+        <f>Z33*AC33</f>
+        <v>40</v>
+      </c>
+      <c r="AI33" s="1"/>
+      <c r="AJ33" s="1"/>
+    </row>
+    <row r="34" spans="25:36" x14ac:dyDescent="0.25">
+      <c r="AI34" s="1"/>
+      <c r="AJ34" s="1"/>
+    </row>
+    <row r="49" spans="35:36" x14ac:dyDescent="0.25">
+      <c r="AI49" s="1"/>
+      <c r="AJ49" s="1"/>
+    </row>
+    <row r="50" spans="35:36" x14ac:dyDescent="0.25">
+      <c r="AI50" s="1"/>
+      <c r="AJ50" s="1"/>
+    </row>
+    <row r="57" spans="35:36" x14ac:dyDescent="0.25">
+      <c r="AI57" s="1"/>
+      <c r="AJ57" s="1"/>
+    </row>
+    <row r="58" spans="35:36" x14ac:dyDescent="0.25">
+      <c r="AI58" s="1"/>
+      <c r="AJ58" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Corrected math in excel file
</commit_message>
<xml_diff>
--- a/Strassen_math.xlsx
+++ b/Strassen_math.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbrin\Documents\GitHub\strassen-snn-accel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B745FB2E-9979-4AEE-83A8-9067C9AAFEE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F42654C-7FD6-4F2A-9A1A-26C34670A987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{612FE5AF-36F0-4BC7-9AAB-A7A5CB9F06BA}"/>
+    <workbookView xWindow="-16320" yWindow="-3600" windowWidth="16440" windowHeight="28320" activeTab="1" xr2:uid="{612FE5AF-36F0-4BC7-9AAB-A7A5CB9F06BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -2859,7 +2859,7 @@
   <dimension ref="E4:AP58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AP24" sqref="AP24"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Wrapper base design works
</commit_message>
<xml_diff>
--- a/Strassen_math.xlsx
+++ b/Strassen_math.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbrin\Documents\GitHub\strassen-snn-accel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19B805F-2F23-44BE-9FAD-B1362041B29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27701435-DCB3-4E9D-AC25-53758772B9C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{612FE5AF-36F0-4BC7-9AAB-A7A5CB9F06BA}"/>
+    <workbookView xWindow="-16305" yWindow="-840" windowWidth="16410" windowHeight="15345" activeTab="1" xr2:uid="{612FE5AF-36F0-4BC7-9AAB-A7A5CB9F06BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -966,7 +966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD2F15B-3E04-4767-9F30-A60E758C5944}">
   <dimension ref="E4:AW60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AH14" sqref="AH14:AH60"/>
     </sheetView>
   </sheetViews>
@@ -3522,8 +3522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC09DD55-F353-4F19-A23A-AFF11BE70FA5}">
   <dimension ref="E4:AP58"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y40" sqref="Y40"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3549,16 +3549,16 @@
     </row>
     <row r="6" spans="5:42" x14ac:dyDescent="0.25">
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>2</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -3568,10 +3568,10 @@
       </c>
       <c r="Q6" cm="1">
         <f t="array" ref="Q6:R7">E8:F9+G8:H9</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="R6">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="T6" t="s">
         <v>10</v>
@@ -3585,11 +3585,11 @@
       </c>
       <c r="Z6">
         <f>Q7+R7</f>
-        <v>58</v>
+        <v>2</v>
       </c>
       <c r="AA6" t="str">
         <f>DEC2HEX(Z6)</f>
-        <v>3A</v>
+        <v>2</v>
       </c>
       <c r="AB6" t="s">
         <v>49</v>
@@ -3607,42 +3607,42 @@
       </c>
       <c r="AF6">
         <f>Z6*AC6</f>
-        <v>58</v>
+        <v>2</v>
       </c>
       <c r="AI6">
         <f>AF7+AF9</f>
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="AM6" cm="1">
         <f t="array" ref="AM6:AM7">AI14:AI15+AI30:AI31</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="AP6" cm="1">
         <f t="array" ref="AP6:AP9">MMULT(E6:H9,J6:J9)</f>
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="5:42" x14ac:dyDescent="0.25">
       <c r="E7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H7">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <v>1</v>
       </c>
       <c r="Q7">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="R7">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="U7">
         <v>1</v>
@@ -3652,11 +3652,11 @@
       </c>
       <c r="Z7">
         <f>Q6</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AA7" t="str">
         <f t="shared" ref="AA7:AA9" si="0">DEC2HEX(Z7)</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="AB7" t="s">
         <v>50</v>
@@ -3678,27 +3678,27 @@
       </c>
       <c r="AI7">
         <f>AF6+AF8</f>
-        <v>58</v>
+        <v>2</v>
       </c>
       <c r="AM7">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="AP7">
-        <v>26</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="5:42" x14ac:dyDescent="0.25">
       <c r="E8">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -3708,11 +3708,11 @@
       </c>
       <c r="Z8">
         <f>R7</f>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="AA8" t="str">
         <f t="shared" si="0"/>
-        <v>1E</v>
+        <v>0</v>
       </c>
       <c r="AB8" t="s">
         <v>51</v>
@@ -3734,24 +3734,24 @@
       </c>
       <c r="AM8" cm="1">
         <f t="array" ref="AM8:AM9">AI6:AI7+AI22:AI23</f>
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="AP8">
-        <v>42</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="5:42" x14ac:dyDescent="0.25">
       <c r="E9">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F9">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -3761,11 +3761,11 @@
       </c>
       <c r="Z9">
         <f>Q6+R6</f>
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="AA9" t="str">
         <f t="shared" si="0"/>
-        <v>2A</v>
+        <v>2</v>
       </c>
       <c r="AB9" t="s">
         <v>52</v>
@@ -3783,15 +3783,15 @@
       </c>
       <c r="AF9">
         <f>Z9*AC9</f>
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="AI9" s="1"/>
       <c r="AJ9" s="1"/>
       <c r="AM9">
-        <v>58</v>
+        <v>2</v>
       </c>
       <c r="AP9">
-        <v>58</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="5:42" x14ac:dyDescent="0.25">
@@ -3825,7 +3825,7 @@
       </c>
       <c r="Q14" cm="1">
         <f t="array" ref="Q14:R15">E6:F7</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R14">
         <v>2</v>
@@ -3842,7 +3842,7 @@
       </c>
       <c r="Z14">
         <f>Q15+R15</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="AB14" t="s">
         <v>69</v>
@@ -3869,10 +3869,10 @@
     </row>
     <row r="15" spans="5:42" x14ac:dyDescent="0.25">
       <c r="Q15">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="R15">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="U15">
         <v>0</v>
@@ -3882,7 +3882,7 @@
       </c>
       <c r="Z15">
         <f>Q14</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB15" t="s">
         <v>70</v>
@@ -3909,7 +3909,7 @@
       </c>
       <c r="Z16">
         <f>R15</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AB16" t="s">
         <v>71</v>
@@ -3932,7 +3932,7 @@
       </c>
       <c r="Z17">
         <f>Q14+R14</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB17" t="s">
         <v>72</v>
@@ -3966,10 +3966,10 @@
       </c>
       <c r="Q22" cm="1">
         <f t="array" ref="Q22:R23">G8:H9</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="R22">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="T22" t="s">
         <v>12</v>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="Z22">
         <f>Q23+R23</f>
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="AB22" t="s">
         <v>90</v>
@@ -4006,10 +4006,10 @@
     </row>
     <row r="23" spans="16:36" x14ac:dyDescent="0.25">
       <c r="Q23">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="R23">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="U23">
         <v>0</v>
@@ -4019,7 +4019,7 @@
       </c>
       <c r="Z23">
         <f>Q22</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="AB23" t="s">
         <v>91</v>
@@ -4046,7 +4046,7 @@
       </c>
       <c r="Z24">
         <f>R23</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="AB24" t="s">
         <v>92</v>
@@ -4069,7 +4069,7 @@
       </c>
       <c r="Z25">
         <f>Q22+R22</f>
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="AB25" t="s">
         <v>93</v>
@@ -4103,10 +4103,10 @@
       </c>
       <c r="Q30" cm="1">
         <f t="array" ref="Q30:R31">E6:F7+G6:H7</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="R30">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="T30" t="s">
         <v>13</v>
@@ -4120,7 +4120,7 @@
       </c>
       <c r="Z30">
         <f>Q31+R31</f>
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="AB30" t="s">
         <v>111</v>
@@ -4134,19 +4134,19 @@
       </c>
       <c r="AF30">
         <f>Z30*AC30</f>
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="AI30">
         <f>AF31+AF33</f>
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="16:36" x14ac:dyDescent="0.25">
       <c r="Q31">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="R31">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="U31">
         <v>1</v>
@@ -4156,7 +4156,7 @@
       </c>
       <c r="Z31">
         <f>Q30</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AB31" t="s">
         <v>112</v>
@@ -4174,7 +4174,7 @@
       </c>
       <c r="AI31">
         <f>AF30+AF32</f>
-        <v>26</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="16:36" x14ac:dyDescent="0.25">
@@ -4183,7 +4183,7 @@
       </c>
       <c r="Z32">
         <f>R31</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="AB32" t="s">
         <v>113</v>
@@ -4206,7 +4206,7 @@
       </c>
       <c r="Z33">
         <f>Q30+R30</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="AB33" t="s">
         <v>114</v>
@@ -4220,7 +4220,7 @@
       </c>
       <c r="AF33">
         <f>Z33*AC33</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="AI33" s="1"/>
       <c r="AJ33" s="1"/>

</xml_diff>